<commit_message>
added info-retrieval2.py, moving a half corpus to Temp Corpus
</commit_message>
<xml_diff>
--- a/cosine.xlsx
+++ b/cosine.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>q1</t>
   </si>
   <si>
-    <t>['D2', 0.876602616509877]</t>
-  </si>
-  <si>
-    <t>['D1', 0.7994587191534351]</t>
+    <t>['D20', 0.35873146904102804]</t>
   </si>
 </sst>
 </file>
@@ -354,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -368,11 +365,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>